<commit_message>
- Calculators are now available offline - Made changes to AC Management recommendations; detailed in AC_Disclaimers.md
</commit_message>
<xml_diff>
--- a/assets/Coag_Options.xlsx
+++ b/assets/Coag_Options.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\FlutterDev\Projects\wikianesthesia_mobile\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D3E1699-FA2D-4288-AE31-C7A9566AA603}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C171EAC7-C210-4537-A3D1-0725F3416FBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{E3ABA24A-03FE-4A22-9483-59CCD4DCB6EA}"/>
   </bookViews>
@@ -304,10 +304,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -651,7 +650,7 @@
   <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -662,16 +661,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="4" t="s">
         <v>49</v>
       </c>
       <c r="E1" s="1" t="s">
@@ -679,300 +678,300 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="D2" s="6">
+      <c r="D2" s="5">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="D3" s="6">
+      <c r="D3" s="5">
         <v>2</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" s="2" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="D4" s="2">
+      <c r="D4">
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="D5" s="2">
+      <c r="D5">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="6" t="s">
+      <c r="A6" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="D6" s="2">
+      <c r="D6">
         <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="6" t="s">
+      <c r="A7" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C7" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="D7" s="2">
+      <c r="D7">
         <v>2</v>
       </c>
-      <c r="E7" s="3" t="s">
+      <c r="E7" s="2" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="B8" s="6" t="s">
+      <c r="A8" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B8" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="C8" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="D8" s="2">
+      <c r="D8">
         <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="6" t="s">
+      <c r="A9" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="B9" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="C9" s="6" t="s">
+      <c r="C9" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="D9" s="2">
+      <c r="D9">
         <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="6" t="s">
+      <c r="A10" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="B10" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="C10" s="6" t="s">
+      <c r="C10" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="D10" s="2">
+      <c r="D10">
         <v>2</v>
       </c>
-      <c r="E10" s="2" t="s">
+      <c r="E10" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="6" t="s">
+      <c r="A11" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="6" t="s">
+      <c r="B11" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="C11" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="D11" s="2">
+      <c r="D11">
         <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="6" t="s">
+      <c r="A12" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="B12" s="6" t="s">
+      <c r="B12" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="C12" s="6" t="s">
+      <c r="C12" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="D12" s="2">
+      <c r="D12">
         <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="6" t="s">
+      <c r="A13" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="B13" s="6" t="s">
+      <c r="B13" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="C13" s="6" t="s">
+      <c r="C13" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="D13" s="2">
+      <c r="D13">
         <v>2</v>
       </c>
-      <c r="E13" s="2" t="s">
+      <c r="E13" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="6" t="s">
+      <c r="A14" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B14" s="6" t="s">
+      <c r="B14" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="C14" s="6" t="s">
+      <c r="C14" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="D14" s="2">
+      <c r="D14">
         <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="6" t="s">
+      <c r="A15" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B15" s="6" t="s">
+      <c r="B15" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="C15" s="6" t="s">
+      <c r="C15" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="D15" s="2">
+      <c r="D15">
         <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="6" t="s">
+      <c r="A16" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="B16" s="6" t="s">
+      <c r="B16" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C16" s="6" t="s">
+      <c r="C16" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="D16" s="2">
+      <c r="D16">
         <v>2</v>
       </c>
-      <c r="E16" s="2" t="s">
+      <c r="E16" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="6" t="s">
+      <c r="A17" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="B17" t="s">
         <v>26</v>
       </c>
-      <c r="C17" s="6" t="s">
+      <c r="C17" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="D17" s="2">
+      <c r="D17">
         <v>3</v>
       </c>
-      <c r="E17" s="2" t="s">
+      <c r="E17" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="6" t="s">
+      <c r="A18" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B18" s="6" t="s">
+      <c r="B18" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="C18" s="6" t="s">
+      <c r="C18" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="D18" s="2">
+      <c r="D18">
         <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="6" t="s">
+      <c r="A19" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B19" s="6" t="s">
+      <c r="B19" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="C19" s="6" t="s">
+      <c r="C19" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="D19" s="2">
+      <c r="D19">
         <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="6" t="s">
+      <c r="A20" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B20" s="6" t="s">
+      <c r="B20" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="C20" s="6" t="s">
+      <c r="C20" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="D20" s="2">
+      <c r="D20">
         <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="6" t="s">
+      <c r="A21" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B21" s="6" t="s">
+      <c r="B21" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="C21" s="6" t="s">
+      <c r="C21" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="D21" s="2">
+      <c r="D21">
         <v>1</v>
       </c>
     </row>

</xml_diff>